<commit_message>
adicionado todos testes de mesa
</commit_message>
<xml_diff>
--- a/testeDMesa.xlsx
+++ b/testeDMesa.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Lado</t>
+    <t>tempo</t>
   </si>
   <si>
-    <t>Area</t>
+    <t>velocidade</t>
+  </si>
+  <si>
+    <t>litros</t>
   </si>
   <si>
     <t>Massa de Dados</t>
@@ -33,9 +36,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -55,15 +58,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -78,6 +89,96 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -85,121 +186,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,7 +211,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.6"/>
+        <fgColor theme="4" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +223,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,19 +235,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,13 +343,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,13 +355,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,6 +367,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -304,109 +403,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,18 +443,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,6 +467,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -492,13 +500,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,150 +529,135 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -669,10 +666,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -682,7 +679,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,15 +687,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1023,74 +1011,91 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="11.25" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="3" width="14.8571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>60</v>
+      </c>
       <c r="C2" s="2">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <f>(B1*B2)/12</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>60</v>
+      </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2">
+      <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>50</v>
+      </c>
       <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>